<commit_message>
code associate and transcrio
</commit_message>
<xml_diff>
--- a/associate_degree.xlsx
+++ b/associate_degree.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="137">
   <si>
     <t>Student Id</t>
   </si>
@@ -439,13 +439,19 @@
   </si>
   <si>
     <t>16th March 2025</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>01.08.20026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -508,8 +514,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,8 +578,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -664,11 +690,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -749,8 +799,14 @@
     <xf numFmtId="49" fontId="6" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -972,9 +1028,9 @@
   </sheetPr>
   <dimension ref="A1:W910"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -991,7 +1047,8 @@
     <col min="10" max="10" width="18.08984375" customWidth="1"/>
     <col min="11" max="11" width="21.1796875" customWidth="1"/>
     <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="18" width="8.6328125" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" customWidth="1"/>
+    <col min="14" max="18" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1031,7 +1088,9 @@
       <c r="L1" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="2"/>
+      <c r="M1" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -1080,6 +1139,9 @@
       <c r="L2" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M2" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
@@ -1118,6 +1180,9 @@
       <c r="L3" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M3" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
@@ -1156,6 +1221,9 @@
       <c r="L4" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M4" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="5" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
@@ -1194,6 +1262,9 @@
       <c r="L5" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M5" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25" t="s">
@@ -1232,6 +1303,9 @@
       <c r="L6" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M6" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="25" t="s">
@@ -1270,6 +1344,9 @@
       <c r="L7" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M7" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="25" t="s">
@@ -1308,6 +1385,9 @@
       <c r="L8" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M8" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="25" t="s">
@@ -1346,6 +1426,9 @@
       <c r="L9" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M9" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="25" t="s">
@@ -1384,6 +1467,9 @@
       <c r="L10" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M10" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25" t="s">
@@ -1422,6 +1508,9 @@
       <c r="L11" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M11" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
@@ -1460,6 +1549,9 @@
       <c r="L12" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M12" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="25" t="s">
@@ -1498,6 +1590,9 @@
       <c r="L13" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M13" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
@@ -1536,6 +1631,9 @@
       <c r="L14" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M14" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="25" t="s">
@@ -1574,6 +1672,9 @@
       <c r="L15" s="28" t="s">
         <v>134</v>
       </c>
+      <c r="M15" s="29" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="26" t="s">
@@ -1612,8 +1713,11 @@
       <c r="L16" s="28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M16" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="26" t="s">
         <v>45</v>
       </c>
@@ -1650,8 +1754,11 @@
       <c r="L17" s="28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M17" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="26" t="s">
         <v>46</v>
       </c>
@@ -1688,8 +1795,11 @@
       <c r="L18" s="28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M18" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="26" t="s">
         <v>47</v>
       </c>
@@ -1726,8 +1836,11 @@
       <c r="L19" s="28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M19" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="26" t="s">
         <v>48</v>
       </c>
@@ -1764,8 +1877,11 @@
       <c r="L20" s="28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M20" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
@@ -1775,7 +1891,7 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
@@ -1785,7 +1901,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
@@ -1795,7 +1911,7 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
@@ -1805,7 +1921,7 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
@@ -1815,7 +1931,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
@@ -1825,7 +1941,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="4"/>
@@ -1835,7 +1951,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="4"/>
@@ -1845,7 +1961,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="4"/>
@@ -1855,7 +1971,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
@@ -1865,7 +1981,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="4"/>
@@ -1875,7 +1991,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="4"/>

</xml_diff>